<commit_message>
Remove flexibility point system (#232)
</commit_message>
<xml_diff>
--- a/InputData/elec/BPaFF/Boolean Peaking and Flexibility Flags.xlsx
+++ b/InputData/elec/BPaFF/Boolean Peaking and Flexibility Flags.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\BPaFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5756EDAE-0404-4F82-907D-D6FB307B7B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E5B677-EBF6-4668-95CF-6FD72EA5F6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30930" yWindow="795" windowWidth="22230" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5235" yWindow="2985" windowWidth="38115" windowHeight="20370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BPaFF-BITPTaP" sheetId="2" r:id="rId2"/>
-    <sheet name="BPaFF-BDTPTPF" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Source:</t>
   </si>
@@ -75,18 +74,9 @@
     <t>BPaFF Boolean Is This Plant Type a Peaker</t>
   </si>
   <si>
-    <t>BPaFF Boolean Does This Plant Type Provide Flexibility</t>
-  </si>
-  <si>
     <t>These variables are used to customize which plant types are used</t>
   </si>
   <si>
-    <t>to satisfy peaking needs and which provide flexibility points, which</t>
-  </si>
-  <si>
-    <t>support renewables in the EPS.</t>
-  </si>
-  <si>
     <t>Peaker plants:</t>
   </si>
   <si>
@@ -105,39 +95,6 @@
     <t>reasons other than their cost-effectiveness.</t>
   </si>
   <si>
-    <t>Plants that provide flexibility:</t>
-  </si>
-  <si>
-    <t>Provide flexibility points based on installed capacity.</t>
-  </si>
-  <si>
-    <t>Generally, the same plants that are flagged as peakers should</t>
-  </si>
-  <si>
-    <t>also be flagged as flexibility providers, and vice versa.</t>
-  </si>
-  <si>
-    <t>However, some countries might aggressively ramp plants</t>
-  </si>
-  <si>
-    <t>that are normally used for baseload, such as coal or</t>
-  </si>
-  <si>
-    <t>nuclear, to provide flexibility.   However, these plants</t>
-  </si>
-  <si>
-    <t>still don't generally get built to satisfy peaking needs</t>
-  </si>
-  <si>
-    <t>and shouldn't be guaranteed a minimum dispatch quantity.</t>
-  </si>
-  <si>
-    <t>These plants should be flagged as flexibility providers but</t>
-  </si>
-  <si>
-    <t>not as peakers.</t>
-  </si>
-  <si>
     <t>lignite</t>
   </si>
   <si>
@@ -163,6 +120,9 @@
   </si>
   <si>
     <t>natural gas combined cycle</t>
+  </si>
+  <si>
+    <t>to satisfy peaking needs, which support renewables in the EPS.</t>
   </si>
 </sst>
 </file>
@@ -552,7 +512,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -563,132 +523,64 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>33</v>
-      </c>
+      <c r="A15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -717,7 +609,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -725,7 +617,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -733,7 +625,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -757,7 +649,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -813,7 +705,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <f>B2</f>
@@ -822,7 +714,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <f>B7</f>
@@ -831,7 +723,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <f>B12</f>
@@ -840,7 +732,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <f>B12</f>
@@ -849,172 +741,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18">
-        <f>B10</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:B18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14">
-        <f>B2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15">
-        <f>B7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16">
-        <f>B12</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17">
-        <f>B12</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <f>B10</f>

</xml_diff>